<commit_message>
coba terbaru nanti aku cek lagi
</commit_message>
<xml_diff>
--- a/downloads/Nh-T.xlsx
+++ b/downloads/Nh-T.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,16 +441,6 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Target Suhu</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Label Jumlah Awan</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
           <t>Prediksi Suhu</t>
         </is>
       </c>
@@ -460,13 +450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>29.71184625</v>
+        <v>29.71184433</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +458,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="n">
-        <v>32</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>29.71184625</v>
+        <v>29.71182699</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +466,7 @@
         <v>89</v>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
-      </c>
-      <c r="C4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>29.71183277</v>
+        <v>29.71167492</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +474,7 @@
         <v>100</v>
       </c>
       <c r="B5" t="n">
-        <v>31</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>29.71184433</v>
+        <v>29.71165378</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +482,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>34</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>29.7118424</v>
+        <v>29.71180773</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +490,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>29</v>
-      </c>
-      <c r="C7" t="n">
-        <v>8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>29.71183084</v>
+        <v>29.71184625</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +498,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="n">
-        <v>28</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>29.71184047</v>
+        <v>29.71176921</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +506,7 @@
         <v>0.9</v>
       </c>
       <c r="B9" t="n">
-        <v>27</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>29.71184625</v>
+        <v>29.71184452</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +514,7 @@
         <v>30</v>
       </c>
       <c r="B10" t="n">
-        <v>25</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="n">
-        <v>29.7118424</v>
+        <v>29.71178847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>